<commit_message>
Archivos para subida .R
</commit_message>
<xml_diff>
--- a/SegundaCompetencia_corridas/HT5230_00_z523.xlsx
+++ b/SegundaCompetencia_corridas/HT5230_00_z523.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiba\Documents\DMenEyF\dmeyf2023\SegundaCompetencia_corridas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC76FC-21E7-43E9-A7CE-9CFA4732B8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E958F7EB-27C4-487A-B8DF-7DD9B6E56961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4815" windowWidth="29040" windowHeight="15840" xr2:uid="{AE2E4154-6A07-481E-AC9D-97EF5200D1B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AE2E4154-6A07-481E-AC9D-97EF5200D1B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="235">
   <si>
     <t>fecha</t>
   </si>
@@ -734,25 +734,13 @@
     <t>KA5240_00__03_z524_lightgbm_final</t>
   </si>
   <si>
-    <t>KA5240_00__04_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__05_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__06_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__07_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__08_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__09_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__10_z524_lightgbm_final</t>
+    <t>KA5240_00 y luego num envios</t>
+  </si>
+  <si>
+    <t>KA5240_00__z524_lightgbm_final</t>
+  </si>
+  <si>
+    <t>Con estos hiperparametros se crrio</t>
   </si>
 </sst>
 </file>
@@ -783,12 +771,18 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -803,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -812,6 +806,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CB4F13-ECDC-4F18-88F4-E4DEC96F6BEC}">
-  <dimension ref="A1:W103"/>
+  <dimension ref="A1:AF103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1149,7 +1144,7 @@
     <col min="18" max="18" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:32">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1183,10 +1178,10 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
@@ -1195,19 +1190,19 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="U1" t="s">
@@ -1217,7 +1212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:32">
       <c r="A2" s="1">
         <v>20230922</v>
       </c>
@@ -1287,8 +1282,17 @@
       <c r="W2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="Z2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
       <c r="A3" s="1">
         <v>20230922</v>
       </c>
@@ -1359,7 +1363,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:32">
       <c r="A4" s="1">
         <v>20230922</v>
       </c>
@@ -1430,7 +1434,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:32">
       <c r="A5" s="1">
         <v>20230922</v>
       </c>
@@ -1497,11 +1501,8 @@
       <c r="V5">
         <v>34</v>
       </c>
-      <c r="W5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
+    </row>
+    <row r="6" spans="1:32">
       <c r="A6" s="1">
         <v>20230922</v>
       </c>
@@ -1568,11 +1569,8 @@
       <c r="V6">
         <v>49</v>
       </c>
-      <c r="W6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23">
+    </row>
+    <row r="7" spans="1:32">
       <c r="A7" s="1">
         <v>20230922</v>
       </c>
@@ -1639,11 +1637,8 @@
       <c r="V7">
         <v>95</v>
       </c>
-      <c r="W7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
+    </row>
+    <row r="8" spans="1:32">
       <c r="A8" s="1">
         <v>20230922</v>
       </c>
@@ -1710,11 +1705,8 @@
       <c r="V8">
         <v>86</v>
       </c>
-      <c r="W8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23">
+    </row>
+    <row r="9" spans="1:32">
       <c r="A9" s="1">
         <v>20230923</v>
       </c>
@@ -1781,11 +1773,8 @@
       <c r="V9">
         <v>101</v>
       </c>
-      <c r="W9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" s="3" customFormat="1">
+    </row>
+    <row r="10" spans="1:32" s="3" customFormat="1">
       <c r="A10" s="2">
         <v>20230922</v>
       </c>
@@ -1853,7 +1842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:32">
       <c r="A11" s="1">
         <v>20230922</v>
       </c>
@@ -1920,11 +1909,8 @@
       <c r="V11">
         <v>61</v>
       </c>
-      <c r="W11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
+    </row>
+    <row r="12" spans="1:32">
       <c r="A12" s="1">
         <v>20230922</v>
       </c>
@@ -1991,11 +1977,8 @@
       <c r="V12">
         <v>46</v>
       </c>
-      <c r="W12" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23">
+    </row>
+    <row r="13" spans="1:32">
       <c r="A13" s="1">
         <v>20230922</v>
       </c>
@@ -2063,7 +2046,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:32">
       <c r="A14" s="1">
         <v>20230922</v>
       </c>
@@ -2131,7 +2114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:32">
       <c r="A15" s="1">
         <v>20230922</v>
       </c>
@@ -2199,7 +2182,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:32">
       <c r="A16" s="1">
         <v>20230922</v>
       </c>

</xml_diff>

<commit_message>
Subimos SQL de FE
</commit_message>
<xml_diff>
--- a/SegundaCompetencia_corridas/HT5230_00_z523.xlsx
+++ b/SegundaCompetencia_corridas/HT5230_00_z523.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiba\Documents\DMenEyF\dmeyf2023\SegundaCompetencia_corridas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E958F7EB-27C4-487A-B8DF-7DD9B6E56961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A52DDE0-81F3-4FA4-AE24-B8546FCD5299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AE2E4154-6A07-481E-AC9D-97EF5200D1B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AE2E4154-6A07-481E-AC9D-97EF5200D1B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="KA5240_00" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -725,22 +726,22 @@
     <t>0.823417447471319</t>
   </si>
   <si>
-    <t>KA5240_00__01_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__02_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__03_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00 y luego num envios</t>
-  </si>
-  <si>
     <t>KA5240_00__z524_lightgbm_final</t>
   </si>
   <si>
     <t>Con estos hiperparametros se crrio</t>
+  </si>
+  <si>
+    <t>Envios</t>
+  </si>
+  <si>
+    <t>KA5240_00_14993</t>
+  </si>
+  <si>
+    <t>Y luego por envios….</t>
+  </si>
+  <si>
+    <t>Public Score</t>
   </si>
 </sst>
 </file>
@@ -833,6 +834,981 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>KA5240_00!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Public Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>KA5240_00!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14993</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>KA5240_00!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>137.47999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131.46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>129.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75DF-4EB4-BEEB-54D95098CB6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1340653600"/>
+        <c:axId val="1859774752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1340653600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="8000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1859774752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1859774752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1340653600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>977612</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>41996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>593148</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC78AE3-96A8-CB52-D01A-077A622013EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1134,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CB4F13-ECDC-4F18-88F4-E4DEC96F6BEC}">
   <dimension ref="A1:AF103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1280,16 +2256,16 @@
         <v>93</v>
       </c>
       <c r="W2" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC2" t="s">
         <v>229</v>
       </c>
-      <c r="Z2" t="s">
-        <v>232</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>233</v>
-      </c>
       <c r="AF2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -1359,9 +2335,6 @@
       <c r="V3">
         <v>65</v>
       </c>
-      <c r="W3" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="1">
@@ -1429,9 +2402,6 @@
       </c>
       <c r="V4">
         <v>59</v>
-      </c>
-      <c r="W4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -8175,4 +9145,143 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1DAAA9-F623-47AD-997E-EE03ED7C5551}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>8000</v>
+      </c>
+      <c r="B2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>9000</v>
+      </c>
+      <c r="B3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>10000</v>
+      </c>
+      <c r="B4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>11000</v>
+      </c>
+      <c r="B5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>11500</v>
+      </c>
+      <c r="B6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>12000</v>
+      </c>
+      <c r="B7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>12500</v>
+      </c>
+      <c r="B8">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4">
+        <v>13000</v>
+      </c>
+      <c r="B9" s="4">
+        <v>135.69999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>13500</v>
+      </c>
+      <c r="B10">
+        <v>137.47999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>14000</v>
+      </c>
+      <c r="B11">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>14500</v>
+      </c>
+      <c r="B12">
+        <v>131.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>14993</v>
+      </c>
+      <c r="B13">
+        <v>129.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>15000</v>
+      </c>
+      <c r="B14">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>16000</v>
+      </c>
+      <c r="B15">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
+    <sortCondition ref="A1:A15"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
auto commit 1       20230928 202419
</commit_message>
<xml_diff>
--- a/SegundaCompetencia_corridas/HT5230_00_z523.xlsx
+++ b/SegundaCompetencia_corridas/HT5230_00_z523.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiba\Documents\DMenEyF\dmeyf2023\SegundaCompetencia_corridas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E958F7EB-27C4-487A-B8DF-7DD9B6E56961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A52DDE0-81F3-4FA4-AE24-B8546FCD5299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AE2E4154-6A07-481E-AC9D-97EF5200D1B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AE2E4154-6A07-481E-AC9D-97EF5200D1B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="KA5240_00" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -725,22 +726,22 @@
     <t>0.823417447471319</t>
   </si>
   <si>
-    <t>KA5240_00__01_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__02_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00__03_z524_lightgbm_final</t>
-  </si>
-  <si>
-    <t>KA5240_00 y luego num envios</t>
-  </si>
-  <si>
     <t>KA5240_00__z524_lightgbm_final</t>
   </si>
   <si>
     <t>Con estos hiperparametros se crrio</t>
+  </si>
+  <si>
+    <t>Envios</t>
+  </si>
+  <si>
+    <t>KA5240_00_14993</t>
+  </si>
+  <si>
+    <t>Y luego por envios….</t>
+  </si>
+  <si>
+    <t>Public Score</t>
   </si>
 </sst>
 </file>
@@ -833,6 +834,981 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>KA5240_00!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Public Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>KA5240_00!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14993</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>KA5240_00!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>137.47999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131.46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>129.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75DF-4EB4-BEEB-54D95098CB6C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1340653600"/>
+        <c:axId val="1859774752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1340653600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="8000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1859774752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1859774752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1340653600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>977612</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>41996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>593148</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC78AE3-96A8-CB52-D01A-077A622013EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1134,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CB4F13-ECDC-4F18-88F4-E4DEC96F6BEC}">
   <dimension ref="A1:AF103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1280,16 +2256,16 @@
         <v>93</v>
       </c>
       <c r="W2" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC2" t="s">
         <v>229</v>
       </c>
-      <c r="Z2" t="s">
-        <v>232</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>233</v>
-      </c>
       <c r="AF2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -1359,9 +2335,6 @@
       <c r="V3">
         <v>65</v>
       </c>
-      <c r="W3" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="1">
@@ -1429,9 +2402,6 @@
       </c>
       <c r="V4">
         <v>59</v>
-      </c>
-      <c r="W4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -8175,4 +9145,143 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1DAAA9-F623-47AD-997E-EE03ED7C5551}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>8000</v>
+      </c>
+      <c r="B2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>9000</v>
+      </c>
+      <c r="B3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>10000</v>
+      </c>
+      <c r="B4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>11000</v>
+      </c>
+      <c r="B5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>11500</v>
+      </c>
+      <c r="B6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>12000</v>
+      </c>
+      <c r="B7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>12500</v>
+      </c>
+      <c r="B8">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4">
+        <v>13000</v>
+      </c>
+      <c r="B9" s="4">
+        <v>135.69999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>13500</v>
+      </c>
+      <c r="B10">
+        <v>137.47999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>14000</v>
+      </c>
+      <c r="B11">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>14500</v>
+      </c>
+      <c r="B12">
+        <v>131.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>14993</v>
+      </c>
+      <c r="B13">
+        <v>129.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>15000</v>
+      </c>
+      <c r="B14">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>16000</v>
+      </c>
+      <c r="B15">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
+    <sortCondition ref="A1:A15"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>